<commit_message>
Ajustes en listados, Carga masiva de areas modificada
</commit_message>
<xml_diff>
--- a/bin/Debug/Archivos/Areas.xlsx
+++ b/bin/Debug/Archivos/Areas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Documents\LICSU\SGSST - TAREAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Documents\LICSU\Archivos Excel Ultimos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0A7B4C-F176-4D6B-9110-BA0D8932A689}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6883C91-24C7-41B7-AE48-91D5033AE92D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AEC2CE36-B28A-449B-A4F8-CFC0393FC9D2}"/>
   </bookViews>
@@ -35,7 +35,31 @@
     <author>Sebastian</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{8E170BD9-3B32-4652-A96F-5E96A9D4C37D}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E89D2F6A-6803-40AB-82F9-8BD0EA0D6DC8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Operativa o Administrativa</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8E170BD9-3B32-4652-A96F-5E96A9D4C37D}">
       <text>
         <r>
           <rPr>
@@ -59,50 +83,41 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00313797-8EDF-478D-B68C-D03A15691590}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Sebastian:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Nivel del area en el organigrama de la empresa (1, 2, 3…)</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
   <si>
-    <t>Area Prueba</t>
-  </si>
-  <si>
     <t>Nombre de Area Padre</t>
   </si>
   <si>
-    <t>Nivel</t>
-  </si>
-  <si>
     <t>Ninguna</t>
+  </si>
+  <si>
+    <t>Tipo de Area</t>
+  </si>
+  <si>
+    <t>Operativa</t>
+  </si>
+  <si>
+    <t>Administrativa</t>
+  </si>
+  <si>
+    <t>Área de Mezcla</t>
+  </si>
+  <si>
+    <t>Area PreMezclado</t>
+  </si>
+  <si>
+    <t>Area PreMezclado 2</t>
+  </si>
+  <si>
+    <t>Area PruebAdmin</t>
   </si>
 </sst>
 </file>
@@ -499,17 +514,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9C1438-49B5-4B83-BFD9-D2B49C7272F8}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -517,25 +531,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>1</v>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>